<commit_message>
treasureManager & prepare rebuild storeItem structure
</commit_message>
<xml_diff>
--- a/Data/SkillDefine.xlsx
+++ b/Data/SkillDefine.xlsx
@@ -1701,8 +1701,8 @@
   <sheetPr/>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -2297,7 +2297,7 @@
         <v>4</v>
       </c>
       <c r="D16">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>-1</v>
@@ -2335,7 +2335,7 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <v>-1</v>
@@ -2753,7 +2753,7 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>-1</v>
@@ -2791,7 +2791,7 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>-1</v>
@@ -2829,7 +2829,7 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>-1</v>
@@ -2905,7 +2905,7 @@
         <v>1</v>
       </c>
       <c r="D32">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <v>-1</v>
@@ -3019,7 +3019,7 @@
         <v>2</v>
       </c>
       <c r="D35">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>-1</v>
@@ -3057,7 +3057,7 @@
         <v>2</v>
       </c>
       <c r="D36">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E36">
         <v>-1</v>
@@ -3095,7 +3095,7 @@
         <v>2</v>
       </c>
       <c r="D37">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>-1</v>
@@ -3133,7 +3133,7 @@
         <v>2</v>
       </c>
       <c r="D38">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>-1</v>
@@ -3171,7 +3171,7 @@
         <v>2</v>
       </c>
       <c r="D39">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E39">
         <v>-1</v>
@@ -3209,7 +3209,7 @@
         <v>3</v>
       </c>
       <c r="D40">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40">
         <v>-1</v>
@@ -3247,10 +3247,10 @@
         <v>3</v>
       </c>
       <c r="D41">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>-1</v>
+        <v>16</v>
       </c>
       <c r="F41">
         <v>10</v>
@@ -3285,7 +3285,7 @@
         <v>3</v>
       </c>
       <c r="D42">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E42">
         <v>-1</v>
@@ -3323,7 +3323,7 @@
         <v>3</v>
       </c>
       <c r="D43">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E43">
         <v>-1</v>
@@ -3361,7 +3361,7 @@
         <v>3</v>
       </c>
       <c r="D44">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E44">
         <v>-1</v>

</xml_diff>